<commit_message>
Added the Group By's, Plots and CAGR Function to the Report Document
</commit_message>
<xml_diff>
--- a/data/min_negative_supplies.xlsx
+++ b/data/min_negative_supplies.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Frequency of Negative Supply</t>
+          <t>Frequency of Negative Supply Months</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
         <v>-161.05</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -506,7 +506,7 @@
         <v>-0.1</v>
       </c>
       <c r="D4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>